<commit_message>
podwójny wykres w excelu
</commit_message>
<xml_diff>
--- a/zad2/MIASI-2.xlsx
+++ b/zad2/MIASI-2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neufrin\Documents\MiASI\zad2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Łukasz\Documents\MiASI\zad2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -94,7 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -112,7 +112,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -144,7 +144,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Wykres oczekiwań w kolejce</a:t>
+              <a:t>Wykres </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -182,37 +182,27 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>w kolejce</c:v>
+          </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$B$14:$B$21</c:f>
               <c:numCache>
@@ -244,8 +234,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$14:$D$21</c:f>
               <c:numCache>
@@ -277,8 +267,90 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Obsłużone</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$14:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.99998663020534073</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99997212790031265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99978502089913812</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9962286996687103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97289335095761065</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89863690194393564</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75584697958684188</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56590189168521865</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -288,11 +360,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-862318448"/>
-        <c:axId val="-862323888"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="-862318448"/>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="670648688"/>
+        <c:axId val="663160656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="670648688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,12 +480,15 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-862323888"/>
+        <c:crossAx val="663160656"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="-862323888"/>
+        <c:axId val="663160656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +529,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>(1-P)</a:t>
+                  <a:t>%</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -494,7 +571,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -531,9 +608,9 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-862318448"/>
+        <c:crossAx val="670648688"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -543,6 +620,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1172,9 +1281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1212,7 +1321,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1284,7 +1393,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1437,7 +1546,7 @@
   <dimension ref="B3:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>